<commit_message>
Adicionada parte inicial da Caverna dos Zubats
</commit_message>
<xml_diff>
--- a/Docs/Encounter locations.xlsx
+++ b/Docs/Encounter locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCA58E7-F81A-428E-AF3E-BBDA885A70F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B49D8-C5A4-4B01-BF77-D5DB0DDA354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encounter locations" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="176">
   <si>
     <t>Pokemon</t>
   </si>
@@ -558,6 +558,12 @@
   </si>
   <si>
     <t>Blacephalon</t>
+  </si>
+  <si>
+    <t>Gligar</t>
+  </si>
+  <si>
+    <t>Noibat</t>
   </si>
 </sst>
 </file>
@@ -1459,13 +1465,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
@@ -1498,7 +1504,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>13</c:v>
@@ -2172,16 +2178,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>604470</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>181707</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2930</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>608134</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>102577</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2210,8 +2216,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H82" totalsRowShown="0">
-  <autoFilter ref="B5:H82" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H84" totalsRowShown="0">
+  <autoFilter ref="B5:H84" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -2527,10 +2533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M82"/>
+  <dimension ref="B1:M84"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,6 +2690,9 @@
       <c r="C7" t="s">
         <v>143</v>
       </c>
+      <c r="D7" s="5">
+        <v>0.7</v>
+      </c>
       <c r="E7" t="s">
         <v>142</v>
       </c>
@@ -2964,25 +2973,25 @@
     </row>
     <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="D16" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E16" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F16" t="s">
         <v>141</v>
       </c>
       <c r="G16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>92</v>
@@ -2993,25 +3002,25 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="D17" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F17" t="s">
         <v>141</v>
       </c>
       <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" t="s">
         <v>72</v>
-      </c>
-      <c r="H17" t="s">
-        <v>47</v>
       </c>
       <c r="J17" t="s">
         <v>0</v>
@@ -3028,21 +3037,24 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>147</v>
       </c>
       <c r="D18" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E18" t="s">
         <v>142</v>
       </c>
       <c r="F18" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" t="s">
         <v>47</v>
       </c>
       <c r="J18" t="s">
@@ -3060,10 +3072,10 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D19" s="5">
         <v>0.05</v>
@@ -3072,13 +3084,10 @@
         <v>142</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G19" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J19" t="s">
         <v>96</v>
@@ -3095,23 +3104,25 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="5"/>
+        <v>95</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.05</v>
+      </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F20" t="s">
         <v>141</v>
       </c>
       <c r="G20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H20" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="J20" t="s">
         <v>29</v>
@@ -3128,25 +3139,23 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
+      <c r="D21" s="5"/>
       <c r="E21" t="s">
         <v>79</v>
       </c>
       <c r="F21" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J21" t="s">
         <v>30</v>
@@ -3163,23 +3172,25 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
       <c r="E22" t="s">
         <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G22" t="s">
         <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J22" t="s">
         <v>31</v>
@@ -3196,25 +3207,23 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
         <v>146</v>
       </c>
-      <c r="D23" s="5">
-        <v>0.05</v>
-      </c>
+      <c r="D23" s="5"/>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F23" t="s">
         <v>141</v>
       </c>
       <c r="G23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="J23" t="s">
         <v>32</v>
@@ -3228,13 +3237,13 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D24" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E24" t="s">
         <v>142</v>
@@ -3243,7 +3252,10 @@
         <v>141</v>
       </c>
       <c r="G24" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="H24" t="s">
+        <v>76</v>
       </c>
       <c r="J24" t="s">
         <v>28</v>
@@ -3260,13 +3272,13 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="D25" s="5">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="E25" t="s">
         <v>142</v>
@@ -3275,10 +3287,7 @@
         <v>141</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J25" t="s">
         <v>27</v>
@@ -3292,19 +3301,25 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>44</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0.4</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F26" t="s">
         <v>141</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
       </c>
       <c r="J26" t="s">
         <v>37</v>
@@ -3321,25 +3336,19 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>131</v>
+        <v>160</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0.05</v>
+        <v>146</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G27" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="J27" t="s">
         <v>59</v>
@@ -3356,25 +3365,25 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
         <v>110</v>
       </c>
       <c r="D28" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E28" t="s">
         <v>142</v>
       </c>
       <c r="F28" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="J28" t="s">
         <v>80</v>
@@ -3388,23 +3397,25 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>161</v>
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>146</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>110</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.1</v>
+      </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G29" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J29" t="s">
         <v>81</v>
@@ -3421,7 +3432,7 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
         <v>146</v>
@@ -3454,25 +3465,23 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>17</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="5">
-        <v>0.4</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
         <v>141</v>
       </c>
       <c r="G31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H31" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="J31" t="s">
         <v>83</v>
@@ -3489,25 +3498,25 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>130</v>
+        <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D32" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
         <v>141</v>
       </c>
       <c r="G32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H32" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="J32" t="s">
         <v>84</v>
@@ -3524,10 +3533,10 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D33" s="5">
         <v>0.2</v>
@@ -3539,10 +3548,10 @@
         <v>141</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="J33" t="s">
         <v>85</v>
@@ -3556,22 +3565,25 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D34" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E34" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F34" t="s">
         <v>141</v>
       </c>
       <c r="G34" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="H34" t="s">
+        <v>58</v>
       </c>
       <c r="J34" t="s">
         <v>86</v>
@@ -3588,16 +3600,16 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C35" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="5">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>149</v>
       </c>
       <c r="F35" t="s">
         <v>141</v>
@@ -3605,9 +3617,6 @@
       <c r="G35" t="s">
         <v>50</v>
       </c>
-      <c r="H35" t="s">
-        <v>48</v>
-      </c>
       <c r="J35" t="s">
         <v>87</v>
       </c>
@@ -3620,16 +3629,16 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>127</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="5">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>43</v>
       </c>
       <c r="F36" t="s">
         <v>141</v>
@@ -3637,6 +3646,9 @@
       <c r="G36" t="s">
         <v>50</v>
       </c>
+      <c r="H36" t="s">
+        <v>48</v>
+      </c>
       <c r="J36" t="s">
         <v>88</v>
       </c>
@@ -3652,25 +3664,22 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D37" s="5">
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="F37" t="s">
         <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
-      </c>
-      <c r="H37" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="J37" t="s">
         <v>89</v>
@@ -3687,13 +3696,13 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D38" s="5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E38" t="s">
         <v>142</v>
@@ -3702,7 +3711,10 @@
         <v>141</v>
       </c>
       <c r="G38" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="H38" t="s">
+        <v>76</v>
       </c>
       <c r="J38" t="s">
         <v>90</v>
@@ -3716,25 +3728,22 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="D39" s="5">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F39" t="s">
         <v>141</v>
       </c>
       <c r="G39" t="s">
-        <v>108</v>
-      </c>
-      <c r="H39" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J39" t="s">
         <v>91</v>
@@ -3751,25 +3760,25 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="C40" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="D40" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F40" t="s">
         <v>141</v>
       </c>
       <c r="G40" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="H40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J40" t="s">
         <v>41</v>
@@ -3786,13 +3795,13 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>126</v>
+        <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="D41" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E41" t="s">
         <v>142</v>
@@ -3801,7 +3810,10 @@
         <v>141</v>
       </c>
       <c r="G41" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="H41" t="s">
+        <v>51</v>
       </c>
       <c r="J41" t="s">
         <v>107</v>
@@ -3815,25 +3827,22 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="C42" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F42" t="s">
         <v>141</v>
       </c>
       <c r="G42" t="s">
-        <v>45</v>
-      </c>
-      <c r="H42" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J42" t="s">
         <v>106</v>
@@ -3850,16 +3859,16 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="D43" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F43" t="s">
         <v>141</v>
@@ -3868,32 +3877,35 @@
         <v>45</v>
       </c>
       <c r="H43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D44" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E44" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
         <v>141</v>
       </c>
       <c r="G44" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="H44" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C45" t="s">
         <v>151</v>
@@ -3908,15 +3920,12 @@
         <v>141</v>
       </c>
       <c r="G45" t="s">
-        <v>56</v>
-      </c>
-      <c r="H45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C46" t="s">
         <v>151</v>
@@ -3931,15 +3940,18 @@
         <v>141</v>
       </c>
       <c r="G46" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="H46" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
@@ -3951,12 +3963,15 @@
         <v>141</v>
       </c>
       <c r="G47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
@@ -3968,12 +3983,12 @@
         <v>141</v>
       </c>
       <c r="G48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>27</v>
+        <v>155</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
@@ -3985,38 +4000,35 @@
         <v>141</v>
       </c>
       <c r="G49" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" t="s">
-        <v>146</v>
+        <v>27</v>
       </c>
       <c r="D50" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F50" t="s">
         <v>141</v>
       </c>
       <c r="G50" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D51" s="5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="E51" t="s">
         <v>142</v>
@@ -4025,18 +4037,18 @@
         <v>141</v>
       </c>
       <c r="G51" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D52" s="5">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E52" t="s">
         <v>142</v>
@@ -4045,38 +4057,35 @@
         <v>141</v>
       </c>
       <c r="G52" t="s">
-        <v>76</v>
-      </c>
-      <c r="H52" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="C53" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D53" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E53" t="s">
         <v>142</v>
       </c>
       <c r="F53" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G53" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="H53" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" t="s">
         <v>44</v>
@@ -4088,67 +4097,67 @@
         <v>142</v>
       </c>
       <c r="F54" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G54" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>44</v>
+      </c>
+      <c r="D55" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C56" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D55" s="10">
+      <c r="D56" s="10">
         <v>0.2</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G55" s="2" t="s">
+      <c r="F56" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="H56" s="3" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>122</v>
-      </c>
-      <c r="C56" t="s">
-        <v>150</v>
-      </c>
-      <c r="D56" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="E56" t="s">
-        <v>142</v>
-      </c>
-      <c r="F56" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" t="s">
-        <v>56</v>
-      </c>
-      <c r="H56" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>34</v>
+        <v>122</v>
       </c>
       <c r="C57" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="D57" s="5">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E57" t="s">
         <v>142</v>
@@ -4157,18 +4166,21 @@
         <v>141</v>
       </c>
       <c r="G57" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="H57" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="D58" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E58" t="s">
         <v>142</v>
@@ -4177,61 +4189,61 @@
         <v>141</v>
       </c>
       <c r="G58" t="s">
-        <v>98</v>
-      </c>
-      <c r="H58" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D59" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E59" t="s">
         <v>142</v>
       </c>
       <c r="F59" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G59" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="H59" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="D60" s="5">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E60" t="s">
         <v>142</v>
       </c>
       <c r="F60" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="G60" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D61" s="5">
-        <v>0.3</v>
+        <v>0.04</v>
       </c>
       <c r="E61" t="s">
         <v>142</v>
@@ -4240,18 +4252,18 @@
         <v>141</v>
       </c>
       <c r="G61" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="C62" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D62" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E62" t="s">
         <v>142</v>
@@ -4260,18 +4272,18 @@
         <v>141</v>
       </c>
       <c r="G62" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="C63" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D63" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E63" t="s">
         <v>142</v>
@@ -4280,21 +4292,18 @@
         <v>141</v>
       </c>
       <c r="G63" t="s">
-        <v>50</v>
-      </c>
-      <c r="H63" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>115</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="D64" s="5">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E64" t="s">
         <v>142</v>
@@ -4303,18 +4312,21 @@
         <v>141</v>
       </c>
       <c r="G64" t="s">
-        <v>76</v>
+        <v>50</v>
+      </c>
+      <c r="H64" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D65" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E65" t="s">
         <v>142</v>
@@ -4323,18 +4335,18 @@
         <v>141</v>
       </c>
       <c r="G65" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C66" t="s">
         <v>147</v>
       </c>
       <c r="D66" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E66" t="s">
         <v>142</v>
@@ -4348,10 +4360,10 @@
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67" t="s">
-        <v>44</v>
+        <v>147</v>
       </c>
       <c r="D67" s="5">
         <v>0.1</v>
@@ -4363,15 +4375,12 @@
         <v>141</v>
       </c>
       <c r="G67" t="s">
-        <v>57</v>
-      </c>
-      <c r="H67" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C68" t="s">
         <v>44</v>
@@ -4386,7 +4395,7 @@
         <v>141</v>
       </c>
       <c r="G68" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H68" t="s">
         <v>46</v>
@@ -4394,56 +4403,59 @@
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C69" t="s">
         <v>44</v>
       </c>
       <c r="D69" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E69" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F69" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G69" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H69" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="D70" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F70" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G70" t="s">
-        <v>72</v>
+        <v>60</v>
+      </c>
+      <c r="H70" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C71" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="D71" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E71" t="s">
         <v>142</v>
@@ -4452,41 +4464,44 @@
         <v>141</v>
       </c>
       <c r="G71" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>114</v>
+        <v>175</v>
       </c>
       <c r="C72" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="D72" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E72" t="s">
         <v>142</v>
       </c>
       <c r="F72" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G72" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="H72" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="C73" t="s">
-        <v>164</v>
+        <v>95</v>
+      </c>
+      <c r="D73" s="5">
+        <v>0.2</v>
       </c>
       <c r="E73" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F73" t="s">
         <v>141</v>
@@ -4494,33 +4509,33 @@
       <c r="G73" t="s">
         <v>48</v>
       </c>
-      <c r="H73" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>165</v>
+        <v>114</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>110</v>
+      </c>
+      <c r="D74" s="5">
+        <v>0.1</v>
       </c>
       <c r="E74" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F74" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G74" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="H74" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C75" t="s">
         <v>164</v>
@@ -4532,15 +4547,15 @@
         <v>141</v>
       </c>
       <c r="G75" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="H75" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C76" t="s">
         <v>164</v>
@@ -4552,12 +4567,15 @@
         <v>141</v>
       </c>
       <c r="G76" t="s">
-        <v>60</v>
+        <v>98</v>
+      </c>
+      <c r="H76" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C77" t="s">
         <v>164</v>
@@ -4569,15 +4587,15 @@
         <v>141</v>
       </c>
       <c r="G77" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="H77" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C78" t="s">
         <v>164</v>
@@ -4589,15 +4607,12 @@
         <v>141</v>
       </c>
       <c r="G78" t="s">
-        <v>54</v>
-      </c>
-      <c r="H78" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C79" t="s">
         <v>164</v>
@@ -4609,15 +4624,15 @@
         <v>141</v>
       </c>
       <c r="G79" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H79" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
         <v>164</v>
@@ -4629,15 +4644,15 @@
         <v>141</v>
       </c>
       <c r="G80" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="H80" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C81" t="s">
         <v>164</v>
@@ -4649,15 +4664,15 @@
         <v>141</v>
       </c>
       <c r="G81" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H81" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C82" t="s">
         <v>164</v>
@@ -4669,16 +4684,56 @@
         <v>141</v>
       </c>
       <c r="G82" t="s">
+        <v>45</v>
+      </c>
+      <c r="H82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>172</v>
+      </c>
+      <c r="C83" t="s">
+        <v>164</v>
+      </c>
+      <c r="E83" t="s">
+        <v>79</v>
+      </c>
+      <c r="F83" t="s">
+        <v>141</v>
+      </c>
+      <c r="G83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H83" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>173</v>
+      </c>
+      <c r="C84" t="s">
+        <v>164</v>
+      </c>
+      <c r="E84" t="s">
+        <v>79</v>
+      </c>
+      <c r="F84" t="s">
+        <v>141</v>
+      </c>
+      <c r="G84" t="s">
         <v>56</v>
       </c>
-      <c r="H82" t="s">
+      <c r="H84" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="B1:M2"/>
     <mergeCell ref="J16:M16"/>
-    <mergeCell ref="B1:M2"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="J4:M4"/>
   </mergeCells>
@@ -4696,14 +4751,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09E350B-F8D3-4669-88FA-2F725652E15C}">
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4768,7 +4825,7 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -4786,7 +4843,7 @@
       </c>
       <c r="C9">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4885,7 +4942,7 @@
       </c>
       <c r="C20">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionada quest Infestação de Vibravas
</commit_message>
<xml_diff>
--- a/Docs/Encounter locations.xlsx
+++ b/Docs/Encounter locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032B49D8-C5A4-4B01-BF77-D5DB0DDA354B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD86EDD-E927-4924-8684-BB2B2FB7A807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="177">
   <si>
     <t>Pokemon</t>
   </si>
@@ -564,6 +564,9 @@
   </si>
   <si>
     <t>Noibat</t>
+  </si>
+  <si>
+    <t>Golett</t>
   </si>
 </sst>
 </file>
@@ -781,9 +784,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -801,6 +801,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1471,7 +1474,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
@@ -1480,7 +1483,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>13</c:v>
@@ -2216,8 +2219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H84" totalsRowShown="0">
-  <autoFilter ref="B5:H84" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H85" totalsRowShown="0">
+  <autoFilter ref="B5:H85" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -2533,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M84"/>
+  <dimension ref="B1:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,34 +2561,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="14"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="17"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="16"/>
     </row>
     <row r="3" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4"/>
@@ -2597,15 +2600,15 @@
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
       <c r="J4" s="18" t="s">
         <v>62</v>
       </c>
@@ -2993,12 +2996,12 @@
       <c r="H16" t="s">
         <v>46</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
@@ -4380,10 +4383,10 @@
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
       <c r="C68" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D68" s="5">
         <v>0.1</v>
@@ -4395,15 +4398,15 @@
         <v>141</v>
       </c>
       <c r="G68" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H68" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C69" t="s">
         <v>44</v>
@@ -4418,7 +4421,7 @@
         <v>141</v>
       </c>
       <c r="G69" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H69" t="s">
         <v>46</v>
@@ -4426,56 +4429,59 @@
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="C70" t="s">
         <v>44</v>
       </c>
       <c r="D70" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E70" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F70" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G70" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H70" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>112</v>
+        <v>49</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>44</v>
       </c>
       <c r="D71" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>79</v>
       </c>
       <c r="F71" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G71" t="s">
-        <v>72</v>
+        <v>60</v>
+      </c>
+      <c r="H71" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>175</v>
+        <v>112</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D72" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E72" t="s">
         <v>142</v>
@@ -4484,21 +4490,18 @@
         <v>141</v>
       </c>
       <c r="G72" t="s">
-        <v>108</v>
-      </c>
-      <c r="H72" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>113</v>
+        <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="D73" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E73" t="s">
         <v>142</v>
@@ -4507,55 +4510,58 @@
         <v>141</v>
       </c>
       <c r="G73" t="s">
-        <v>48</v>
+        <v>108</v>
+      </c>
+      <c r="H73" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="D74" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E74" t="s">
         <v>142</v>
       </c>
       <c r="F74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G74" t="s">
-        <v>47</v>
-      </c>
-      <c r="H74" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>163</v>
+        <v>114</v>
       </c>
       <c r="C75" t="s">
-        <v>164</v>
+        <v>110</v>
+      </c>
+      <c r="D75" s="5">
+        <v>0.1</v>
       </c>
       <c r="E75" t="s">
-        <v>79</v>
+        <v>142</v>
       </c>
       <c r="F75" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G75" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H75" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C76" t="s">
         <v>164</v>
@@ -4567,15 +4573,15 @@
         <v>141</v>
       </c>
       <c r="G76" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="H76" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C77" t="s">
         <v>164</v>
@@ -4595,7 +4601,7 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C78" t="s">
         <v>164</v>
@@ -4607,12 +4613,15 @@
         <v>141</v>
       </c>
       <c r="G78" t="s">
-        <v>60</v>
+        <v>98</v>
+      </c>
+      <c r="H78" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
         <v>164</v>
@@ -4624,15 +4633,12 @@
         <v>141</v>
       </c>
       <c r="G79" t="s">
-        <v>51</v>
-      </c>
-      <c r="H79" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C80" t="s">
         <v>164</v>
@@ -4644,15 +4650,15 @@
         <v>141</v>
       </c>
       <c r="G80" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H80" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C81" t="s">
         <v>164</v>
@@ -4664,15 +4670,15 @@
         <v>141</v>
       </c>
       <c r="G81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H81" t="s">
-        <v>108</v>
+        <v>51</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C82" t="s">
         <v>164</v>
@@ -4684,7 +4690,7 @@
         <v>141</v>
       </c>
       <c r="G82" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H82" t="s">
         <v>108</v>
@@ -4692,7 +4698,7 @@
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C83" t="s">
         <v>164</v>
@@ -4704,15 +4710,15 @@
         <v>141</v>
       </c>
       <c r="G83" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H83" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C84" t="s">
         <v>164</v>
@@ -4724,9 +4730,29 @@
         <v>141</v>
       </c>
       <c r="G84" t="s">
+        <v>48</v>
+      </c>
+      <c r="H84" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" t="s">
+        <v>164</v>
+      </c>
+      <c r="E85" t="s">
+        <v>79</v>
+      </c>
+      <c r="F85" t="s">
+        <v>141</v>
+      </c>
+      <c r="G85" t="s">
         <v>56</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H85" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4843,7 +4869,7 @@
       </c>
       <c r="C9">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4870,7 +4896,7 @@
       </c>
       <c r="C12">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualizado tileset dos Esgotos
</commit_message>
<xml_diff>
--- a/Docs/Encounter locations.xlsx
+++ b/Docs/Encounter locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD86EDD-E927-4924-8684-BB2B2FB7A807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6497D74-C98B-41A1-9277-2EC82B4F9E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="177">
   <si>
     <t>Pokemon</t>
   </si>
@@ -83,9 +83,6 @@
     <t>Carvanha</t>
   </si>
   <si>
-    <t>Gulpin</t>
-  </si>
-  <si>
     <t>Cacnea</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>Golett</t>
+  </si>
+  <si>
+    <t>Rattata</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1462,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -1471,7 +1471,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16</c:v>
@@ -1492,7 +1492,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>10</c:v>
@@ -2219,8 +2219,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H85" totalsRowShown="0">
-  <autoFilter ref="B5:H85" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H84" totalsRowShown="0">
+  <autoFilter ref="B5:H84" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -2536,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M85"/>
+  <dimension ref="B1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,7 +2601,7 @@
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -2610,7 +2610,7 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="J4" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -2653,351 +2653,348 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" t="s">
         <v>139</v>
       </c>
-      <c r="C6" t="s">
-        <v>95</v>
-      </c>
       <c r="D6" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
-      </c>
-      <c r="H6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="L6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="D7" s="5">
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="E7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="J7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" t="s">
         <v>74</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" t="s">
         <v>75</v>
-      </c>
-      <c r="L7" t="s">
-        <v>58</v>
-      </c>
-      <c r="M7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
+      <c r="H8" t="s">
+        <v>45</v>
       </c>
       <c r="J8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
+        <v>143</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>43</v>
       </c>
       <c r="D10" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
+        <v>140</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
       </c>
       <c r="J10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" t="s">
         <v>65</v>
       </c>
-      <c r="K10" t="s">
-        <v>66</v>
-      </c>
       <c r="L10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F12" t="s">
+        <v>140</v>
+      </c>
+      <c r="G12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>137</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>43</v>
       </c>
       <c r="D13" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
-      </c>
-      <c r="H13" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="D14" s="5">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="E14" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="J14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K14" t="s">
+        <v>70</v>
+      </c>
+      <c r="L14" t="s">
         <v>71</v>
       </c>
-      <c r="L14" t="s">
-        <v>72</v>
-      </c>
       <c r="M14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>136</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D15" s="5">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="E15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D16" s="5">
         <v>0.1</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
@@ -3005,25 +3002,25 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="C17" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="D17" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="F17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s">
         <v>0</v>
@@ -3040,37 +3037,37 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="D18" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
@@ -3078,31 +3075,34 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="D19" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
       </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
@@ -3110,196 +3110,196 @@
         <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5">
         <v>0.05</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G20" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L20" t="s">
         <v>53</v>
       </c>
-      <c r="J20" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" t="s">
-        <v>99</v>
-      </c>
-      <c r="L20" t="s">
-        <v>54</v>
-      </c>
       <c r="M20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="E21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" t="s">
+        <v>97</v>
+      </c>
+      <c r="M21" t="s">
         <v>44</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>141</v>
-      </c>
-      <c r="G21" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" t="s">
-        <v>98</v>
-      </c>
-      <c r="M21" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" t="s">
+        <v>53</v>
+      </c>
+      <c r="M22" t="s">
         <v>51</v>
-      </c>
-      <c r="H22" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" t="s">
-        <v>31</v>
-      </c>
-      <c r="K22" t="s">
-        <v>99</v>
-      </c>
-      <c r="L22" t="s">
-        <v>54</v>
-      </c>
-      <c r="M22" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D23" s="5">
+        <v>1</v>
+      </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="s">
         <v>51</v>
       </c>
-      <c r="H23" t="s">
-        <v>48</v>
-      </c>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="C24" t="s">
-        <v>146</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.05</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H24" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="J24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D25" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" t="s">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
+        <v>75</v>
       </c>
       <c r="J25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
@@ -3307,720 +3307,726 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D26" s="5">
         <v>0.4</v>
       </c>
       <c r="E26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" s="5">
         <v>0.05</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="5">
         <v>0.1</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M30" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K31" t="s">
+        <v>102</v>
+      </c>
+      <c r="L31" t="s">
         <v>103</v>
       </c>
-      <c r="L31" t="s">
-        <v>104</v>
-      </c>
       <c r="M31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5">
         <v>0.4</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" s="5">
         <v>0.2</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D34" s="5">
         <v>0.2</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K34" t="s">
+        <v>96</v>
+      </c>
+      <c r="L34" t="s">
+        <v>59</v>
+      </c>
+      <c r="M34" t="s">
         <v>97</v>
-      </c>
-      <c r="L34" t="s">
-        <v>60</v>
-      </c>
-      <c r="M34" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D35" s="5">
         <v>0.3</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G35" t="s">
+        <v>49</v>
+      </c>
+      <c r="J35" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" t="s">
+        <v>96</v>
+      </c>
+      <c r="L35" t="s">
         <v>50</v>
-      </c>
-      <c r="J35" t="s">
-        <v>87</v>
-      </c>
-      <c r="K35" t="s">
-        <v>97</v>
-      </c>
-      <c r="L35" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D36" s="5">
         <v>0.17</v>
       </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>47</v>
+      </c>
+      <c r="J36" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" t="s">
+        <v>96</v>
+      </c>
+      <c r="L36" t="s">
         <v>50</v>
       </c>
-      <c r="H36" t="s">
-        <v>48</v>
-      </c>
-      <c r="J36" t="s">
-        <v>88</v>
-      </c>
-      <c r="K36" t="s">
-        <v>97</v>
-      </c>
-      <c r="L36" t="s">
-        <v>51</v>
-      </c>
       <c r="M36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" s="5">
         <v>0.3</v>
       </c>
       <c r="E37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" t="s">
+        <v>88</v>
+      </c>
+      <c r="K37" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" t="s">
+        <v>47</v>
+      </c>
+      <c r="M37" t="s">
         <v>50</v>
-      </c>
-      <c r="J37" t="s">
-        <v>89</v>
-      </c>
-      <c r="K37" t="s">
-        <v>97</v>
-      </c>
-      <c r="L37" t="s">
-        <v>48</v>
-      </c>
-      <c r="M37" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D38" s="5">
         <v>0.01</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="5">
         <v>0.03</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K39" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" s="5">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="5">
         <v>0.05</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J41" t="s">
+        <v>106</v>
+      </c>
+      <c r="K41" t="s">
+        <v>104</v>
+      </c>
+      <c r="L41" t="s">
         <v>107</v>
-      </c>
-      <c r="K41" t="s">
-        <v>105</v>
-      </c>
-      <c r="L41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D42" s="5">
         <v>0.1</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D43" s="5">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D44" s="5">
         <v>0.1</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F44" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D45" s="5">
         <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D46" s="5">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G47" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>155</v>
+        <v>154</v>
+      </c>
+      <c r="C49" t="s">
+        <v>139</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>27</v>
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
+        <v>145</v>
       </c>
       <c r="D50" s="5">
-        <v>1</v>
+        <v>0.05</v>
       </c>
       <c r="E50" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G50" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -4028,19 +4034,19 @@
         <v>123</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D51" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G51" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -4048,42 +4054,45 @@
         <v>124</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="D52" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G52" t="s">
-        <v>48</v>
+        <v>75</v>
+      </c>
+      <c r="H52" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="C53" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D53" s="5">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F53" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G53" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="H53" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -4091,234 +4100,231 @@
         <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D54" s="5">
         <v>0.15</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F54" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>47</v>
-      </c>
-      <c r="H54" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D55" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="E55" t="s">
-        <v>142</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="B55" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G55" t="s">
+      <c r="F55" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D56" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>53</v>
+      <c r="H56" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>122</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="D57" s="5">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="E57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G57" t="s">
-        <v>56</v>
-      </c>
-      <c r="H57" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="D58" s="5">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="E58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G58" t="s">
-        <v>54</v>
+        <v>97</v>
+      </c>
+      <c r="H58" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D59" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E59" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F59" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G59" t="s">
-        <v>98</v>
-      </c>
-      <c r="H59" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>120</v>
+        <v>35</v>
       </c>
       <c r="C60" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="D60" s="5">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F60" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G60" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D61" s="5">
-        <v>0.04</v>
+        <v>0.3</v>
       </c>
       <c r="E61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G61" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D62" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G62" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>147</v>
+        <v>43</v>
       </c>
       <c r="D63" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G63" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="H63" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="C64" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="D64" s="5">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="E64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F64" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G64" t="s">
-        <v>50</v>
-      </c>
-      <c r="H64" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
@@ -4329,16 +4335,16 @@
         <v>146</v>
       </c>
       <c r="D65" s="5">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G65" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
@@ -4346,62 +4352,65 @@
         <v>116</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D66" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G66" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="C67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D67" s="5">
         <v>0.1</v>
       </c>
       <c r="E67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G67" t="s">
-        <v>72</v>
+        <v>46</v>
+      </c>
+      <c r="H67" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D68" s="5">
         <v>0.1</v>
       </c>
       <c r="E68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G68" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H68" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -4409,111 +4418,108 @@
         <v>118</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D69" s="5">
         <v>0.1</v>
       </c>
       <c r="E69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H69" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>119</v>
+        <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D70" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F70" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G70" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="H70" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>49</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="D71" s="5">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="E71" t="s">
-        <v>79</v>
+        <v>141</v>
       </c>
       <c r="F71" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G71" t="s">
-        <v>60</v>
-      </c>
-      <c r="H71" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D72" s="5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="E72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>72</v>
+        <v>107</v>
+      </c>
+      <c r="H72" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>175</v>
+        <v>112</v>
       </c>
       <c r="C73" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="D73" s="5">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="E73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F73" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G73" t="s">
-        <v>108</v>
-      </c>
-      <c r="H73" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
@@ -4521,62 +4527,62 @@
         <v>113</v>
       </c>
       <c r="C74" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D74" s="5">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F74" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G74" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="H74" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>114</v>
+        <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" s="5">
-        <v>0.1</v>
+        <v>163</v>
       </c>
       <c r="E75" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G75" t="s">
         <v>47</v>
       </c>
       <c r="H75" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" t="s">
         <v>163</v>
       </c>
-      <c r="C76" t="s">
-        <v>164</v>
-      </c>
       <c r="E76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G76" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="H76" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
@@ -4584,19 +4590,19 @@
         <v>165</v>
       </c>
       <c r="C77" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G77" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H77" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
@@ -4604,19 +4610,16 @@
         <v>166</v>
       </c>
       <c r="C78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G78" t="s">
-        <v>98</v>
-      </c>
-      <c r="H78" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
@@ -4624,16 +4627,19 @@
         <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E79" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F79" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G79" t="s">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="H79" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
@@ -4641,19 +4647,19 @@
         <v>168</v>
       </c>
       <c r="C80" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F80" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G80" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H80" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
@@ -4661,19 +4667,19 @@
         <v>169</v>
       </c>
       <c r="C81" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G81" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H81" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -4681,19 +4687,19 @@
         <v>170</v>
       </c>
       <c r="C82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E82" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F82" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G82" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
@@ -4701,19 +4707,19 @@
         <v>171</v>
       </c>
       <c r="C83" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G83" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H83" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
@@ -4721,39 +4727,19 @@
         <v>172</v>
       </c>
       <c r="C84" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E84" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F84" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G84" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="H84" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>173</v>
-      </c>
-      <c r="C85" t="s">
-        <v>164</v>
-      </c>
-      <c r="E85" t="s">
-        <v>79</v>
-      </c>
-      <c r="F85" t="s">
-        <v>141</v>
-      </c>
-      <c r="G85" t="s">
-        <v>56</v>
-      </c>
-      <c r="H85" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4791,7 +4777,7 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -4821,24 +4807,24 @@
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4847,7 +4833,7 @@
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4856,16 +4842,16 @@
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4874,7 +4860,7 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4883,7 +4869,7 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4892,7 +4878,7 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4901,7 +4887,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4910,7 +4896,7 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4919,16 +4905,16 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4937,7 +4923,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4946,7 +4932,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4955,7 +4941,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4964,7 +4950,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4973,7 +4959,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
@@ -4982,7 +4968,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>

</xml_diff>

<commit_message>
Adicionados Plasma Shadows nos esgotos
E alguns outros eventos.
</commit_message>
<xml_diff>
--- a/Docs/Encounter locations.xlsx
+++ b/Docs/Encounter locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232097FF-9F03-4FED-949F-7FA34E7057BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99751C37-336B-47BE-86D2-C42518B7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="179">
   <si>
     <t>Pokemon</t>
   </si>
@@ -570,6 +570,9 @@
   </si>
   <si>
     <t xml:space="preserve">Totodile </t>
+  </si>
+  <si>
+    <t>Wooper</t>
   </si>
 </sst>
 </file>
@@ -1477,7 +1480,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>16</c:v>
@@ -1495,7 +1498,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>10</c:v>
@@ -2222,8 +2225,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H85" totalsRowShown="0">
-  <autoFilter ref="B5:H85" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H86" totalsRowShown="0">
+  <autoFilter ref="B5:H86" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -2539,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M85"/>
+  <dimension ref="B1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,25 +3038,23 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C18" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F18" t="s">
         <v>140</v>
       </c>
       <c r="G18" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
         <v>46</v>
-      </c>
-      <c r="H18" t="s">
-        <v>45</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
@@ -3070,25 +3071,25 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
         <v>140</v>
       </c>
       <c r="G19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="J19" t="s">
         <v>95</v>
@@ -3105,25 +3106,25 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
         <v>140</v>
       </c>
       <c r="G20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" t="s">
         <v>71</v>
-      </c>
-      <c r="H20" t="s">
-        <v>46</v>
       </c>
       <c r="J20" t="s">
         <v>28</v>
@@ -3140,21 +3141,24 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="D21" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E21" t="s">
         <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G21" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" t="s">
         <v>46</v>
       </c>
       <c r="J21" t="s">
@@ -3172,10 +3176,10 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D22" s="5">
         <v>0.05</v>
@@ -3184,13 +3188,10 @@
         <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
-      </c>
-      <c r="H22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J22" t="s">
         <v>30</v>
@@ -3207,23 +3208,25 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0.05</v>
+      </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F23" t="s">
         <v>140</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="J23" t="s">
         <v>31</v>
@@ -3237,25 +3240,23 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="5">
-        <v>1</v>
-      </c>
+      <c r="D24" s="5"/>
       <c r="E24" t="s">
         <v>78</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H24" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J24" t="s">
         <v>27</v>
@@ -3272,23 +3273,25 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>158</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
-      </c>
-      <c r="D25" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
       <c r="E25" t="s">
         <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G25" t="s">
         <v>50</v>
       </c>
       <c r="H25" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J25" t="s">
         <v>26</v>
@@ -3302,25 +3305,23 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C26" t="s">
         <v>145</v>
       </c>
-      <c r="D26" s="5">
-        <v>0.05</v>
-      </c>
+      <c r="D26" s="5"/>
       <c r="E26" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F26" t="s">
         <v>140</v>
       </c>
       <c r="G26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="J26" t="s">
         <v>36</v>
@@ -3337,13 +3338,13 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D27" s="5">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="E27" t="s">
         <v>141</v>
@@ -3352,10 +3353,10 @@
         <v>140</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s">
         <v>58</v>
@@ -3372,19 +3373,25 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>145</v>
+        <v>43</v>
+      </c>
+      <c r="D28" s="5">
+        <v>0.4</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F28" t="s">
         <v>140</v>
       </c>
       <c r="G28" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="H28" t="s">
+        <v>52</v>
       </c>
       <c r="J28" t="s">
         <v>79</v>
@@ -3398,25 +3405,19 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0.05</v>
+        <v>145</v>
       </c>
       <c r="E29" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G29" t="s">
-        <v>46</v>
-      </c>
-      <c r="H29" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J29" t="s">
         <v>80</v>
@@ -3433,25 +3434,25 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
         <v>109</v>
       </c>
       <c r="D30" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E30" t="s">
         <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J30" t="s">
         <v>81</v>
@@ -3468,23 +3469,25 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s">
-        <v>145</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="D31" s="5">
+        <v>0.1</v>
+      </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F31" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G31" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H31" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="J31" t="s">
         <v>82</v>
@@ -3501,7 +3504,7 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>145</v>
@@ -3534,25 +3537,23 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="5">
-        <v>0.4</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D33" s="5"/>
       <c r="E33" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
         <v>140</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H33" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="J33" t="s">
         <v>84</v>
@@ -3566,25 +3567,25 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="C34" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D34" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E34" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
         <v>140</v>
       </c>
       <c r="G34" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H34" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="J34" t="s">
         <v>85</v>
@@ -3601,10 +3602,10 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D35" s="5">
         <v>0.2</v>
@@ -3616,10 +3617,10 @@
         <v>140</v>
       </c>
       <c r="G35" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="H35" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J35" t="s">
         <v>86</v>
@@ -3633,22 +3634,25 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="D36" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F36" t="s">
         <v>140</v>
       </c>
       <c r="G36" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="H36" t="s">
+        <v>57</v>
       </c>
       <c r="J36" t="s">
         <v>87</v>
@@ -3665,16 +3669,16 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" t="s">
         <v>43</v>
       </c>
       <c r="D37" s="5">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
       <c r="E37" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="F37" t="s">
         <v>140</v>
@@ -3682,9 +3686,6 @@
       <c r="G37" t="s">
         <v>49</v>
       </c>
-      <c r="H37" t="s">
-        <v>47</v>
-      </c>
       <c r="J37" t="s">
         <v>88</v>
       </c>
@@ -3700,16 +3701,16 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="5">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="E38" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="F38" t="s">
         <v>140</v>
@@ -3717,6 +3718,9 @@
       <c r="G38" t="s">
         <v>49</v>
       </c>
+      <c r="H38" t="s">
+        <v>47</v>
+      </c>
       <c r="J38" t="s">
         <v>89</v>
       </c>
@@ -3729,25 +3733,22 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C39" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D39" s="5">
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="E39" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F39" t="s">
         <v>140</v>
       </c>
       <c r="G39" t="s">
-        <v>50</v>
-      </c>
-      <c r="H39" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="J39" t="s">
         <v>90</v>
@@ -3764,13 +3765,13 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C40" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D40" s="5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E40" t="s">
         <v>141</v>
@@ -3779,7 +3780,10 @@
         <v>140</v>
       </c>
       <c r="G40" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="H40" t="s">
+        <v>75</v>
       </c>
       <c r="J40" t="s">
         <v>40</v>
@@ -3796,25 +3800,22 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="D41" s="5">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E41" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
         <v>140</v>
       </c>
       <c r="G41" t="s">
-        <v>107</v>
-      </c>
-      <c r="H41" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J41" t="s">
         <v>106</v>
@@ -3828,25 +3829,25 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C42" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D42" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F42" t="s">
         <v>140</v>
       </c>
       <c r="G42" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="H42" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J42" t="s">
         <v>105</v>
@@ -3863,13 +3864,13 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="D43" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E43" t="s">
         <v>141</v>
@@ -3878,44 +3879,44 @@
         <v>140</v>
       </c>
       <c r="G43" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="H43" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D44" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F44" t="s">
         <v>140</v>
       </c>
       <c r="G44" t="s">
-        <v>44</v>
-      </c>
-      <c r="H44" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="D45" s="5">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F45" t="s">
         <v>140</v>
@@ -3924,32 +3925,35 @@
         <v>44</v>
       </c>
       <c r="H45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D46" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
         <v>140</v>
       </c>
       <c r="G46" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="H46" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C47" t="s">
         <v>150</v>
@@ -3964,15 +3968,12 @@
         <v>140</v>
       </c>
       <c r="G47" t="s">
-        <v>55</v>
-      </c>
-      <c r="H47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C48" t="s">
         <v>150</v>
@@ -3987,15 +3988,18 @@
         <v>140</v>
       </c>
       <c r="G48" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H48" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
@@ -4007,15 +4011,15 @@
         <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D50" s="5">
         <v>1</v>
@@ -4027,38 +4031,38 @@
         <v>140</v>
       </c>
       <c r="G50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="C51" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D51" s="5">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F51" t="s">
         <v>140</v>
       </c>
       <c r="G51" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D52" s="5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="E52" t="s">
         <v>141</v>
@@ -4067,18 +4071,18 @@
         <v>140</v>
       </c>
       <c r="G52" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D53" s="5">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E53" t="s">
         <v>141</v>
@@ -4087,38 +4091,35 @@
         <v>140</v>
       </c>
       <c r="G53" t="s">
-        <v>75</v>
-      </c>
-      <c r="H53" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D54" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E54" t="s">
         <v>141</v>
       </c>
       <c r="F54" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H54" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55" t="s">
         <v>43</v>
@@ -4130,67 +4131,67 @@
         <v>141</v>
       </c>
       <c r="F55" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G55" t="s">
+        <v>46</v>
+      </c>
+      <c r="H55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E56" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" t="s">
+        <v>140</v>
+      </c>
+      <c r="G56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="10">
+      <c r="D57" s="10">
         <v>0.2</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G56" s="2" t="s">
+      <c r="F57" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H57" s="3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>121</v>
-      </c>
-      <c r="C57" t="s">
-        <v>149</v>
-      </c>
-      <c r="D57" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="E57" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" t="s">
-        <v>140</v>
-      </c>
-      <c r="G57" t="s">
-        <v>55</v>
-      </c>
-      <c r="H57" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="D58" s="5">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E58" t="s">
         <v>141</v>
@@ -4199,18 +4200,21 @@
         <v>140</v>
       </c>
       <c r="G58" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="H58" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D59" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E59" t="s">
         <v>141</v>
@@ -4219,61 +4223,61 @@
         <v>140</v>
       </c>
       <c r="G59" t="s">
-        <v>97</v>
-      </c>
-      <c r="H59" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D60" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E60" t="s">
         <v>141</v>
       </c>
       <c r="F60" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G60" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="H60" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="D61" s="5">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E61" t="s">
         <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G61" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D62" s="5">
-        <v>0.3</v>
+        <v>0.04</v>
       </c>
       <c r="E62" t="s">
         <v>141</v>
@@ -4282,18 +4286,18 @@
         <v>140</v>
       </c>
       <c r="G62" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C63" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D63" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E63" t="s">
         <v>141</v>
@@ -4302,18 +4306,18 @@
         <v>140</v>
       </c>
       <c r="G63" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="D64" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E64" t="s">
         <v>141</v>
@@ -4322,21 +4326,18 @@
         <v>140</v>
       </c>
       <c r="G64" t="s">
-        <v>49</v>
-      </c>
-      <c r="H64" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D65" s="5">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E65" t="s">
         <v>141</v>
@@ -4345,18 +4346,21 @@
         <v>140</v>
       </c>
       <c r="G65" t="s">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="H65" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D66" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E66" t="s">
         <v>141</v>
@@ -4365,18 +4369,18 @@
         <v>140</v>
       </c>
       <c r="G66" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C67" t="s">
         <v>146</v>
       </c>
       <c r="D67" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E67" t="s">
         <v>141</v>
@@ -4390,10 +4394,10 @@
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D68" s="5">
         <v>0.1</v>
@@ -4405,18 +4409,15 @@
         <v>140</v>
       </c>
       <c r="G68" t="s">
-        <v>46</v>
-      </c>
-      <c r="H68" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="C69" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D69" s="5">
         <v>0.1</v>
@@ -4428,15 +4429,15 @@
         <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H69" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" t="s">
         <v>43</v>
@@ -4451,7 +4452,7 @@
         <v>140</v>
       </c>
       <c r="G70" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H70" t="s">
         <v>45</v>
@@ -4459,56 +4460,59 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="C71" t="s">
         <v>43</v>
       </c>
       <c r="D71" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E71" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G71" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H71" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
       <c r="C72" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D72" s="5">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F72" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G72" t="s">
-        <v>71</v>
+        <v>59</v>
+      </c>
+      <c r="H72" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>174</v>
+        <v>111</v>
       </c>
       <c r="C73" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D73" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E73" t="s">
         <v>141</v>
@@ -4517,21 +4521,18 @@
         <v>140</v>
       </c>
       <c r="G73" t="s">
-        <v>107</v>
-      </c>
-      <c r="H73" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>112</v>
+        <v>174</v>
       </c>
       <c r="C74" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="D74" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E74" t="s">
         <v>141</v>
@@ -4540,55 +4541,58 @@
         <v>140</v>
       </c>
       <c r="G74" t="s">
-        <v>47</v>
+        <v>107</v>
+      </c>
+      <c r="H74" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D75" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E75" t="s">
         <v>141</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G75" t="s">
-        <v>46</v>
-      </c>
-      <c r="H75" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="C76" t="s">
-        <v>163</v>
+        <v>109</v>
+      </c>
+      <c r="D76" s="5">
+        <v>0.1</v>
       </c>
       <c r="E76" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F76" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G76" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H76" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C77" t="s">
         <v>163</v>
@@ -4600,15 +4604,15 @@
         <v>140</v>
       </c>
       <c r="G77" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="H77" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" t="s">
         <v>163</v>
@@ -4628,7 +4632,7 @@
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
         <v>163</v>
@@ -4640,12 +4644,15 @@
         <v>140</v>
       </c>
       <c r="G79" t="s">
-        <v>59</v>
+        <v>97</v>
+      </c>
+      <c r="H79" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C80" t="s">
         <v>163</v>
@@ -4657,15 +4664,12 @@
         <v>140</v>
       </c>
       <c r="G80" t="s">
-        <v>50</v>
-      </c>
-      <c r="H80" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C81" t="s">
         <v>163</v>
@@ -4677,15 +4681,15 @@
         <v>140</v>
       </c>
       <c r="G81" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H81" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C82" t="s">
         <v>163</v>
@@ -4697,15 +4701,15 @@
         <v>140</v>
       </c>
       <c r="G82" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H82" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C83" t="s">
         <v>163</v>
@@ -4717,7 +4721,7 @@
         <v>140</v>
       </c>
       <c r="G83" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="H83" t="s">
         <v>107</v>
@@ -4725,7 +4729,7 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C84" t="s">
         <v>163</v>
@@ -4737,15 +4741,15 @@
         <v>140</v>
       </c>
       <c r="G84" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H84" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C85" t="s">
         <v>163</v>
@@ -4757,9 +4761,29 @@
         <v>140</v>
       </c>
       <c r="G85" t="s">
+        <v>47</v>
+      </c>
+      <c r="H85" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" t="s">
+        <v>163</v>
+      </c>
+      <c r="E86" t="s">
+        <v>78</v>
+      </c>
+      <c r="F86" t="s">
+        <v>140</v>
+      </c>
+      <c r="G86" t="s">
         <v>55</v>
       </c>
-      <c r="H85" t="s">
+      <c r="H86" t="s">
         <v>57</v>
       </c>
     </row>
@@ -4876,7 +4900,7 @@
       </c>
       <c r="C9">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4930,7 +4954,7 @@
       </c>
       <c r="C15">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adicionadas salas opcionais da Relic Passage
</commit_message>
<xml_diff>
--- a/Docs/Encounter locations.xlsx
+++ b/Docs/Encounter locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benit\Documents\GitHub\Pokemon Burning Scales\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99751C37-336B-47BE-86D2-C42518B7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DB27E1C-B80D-49C2-A666-A6357C3F5CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="173">
   <si>
     <t>Pokemon</t>
   </si>
@@ -524,39 +524,6 @@
     <t>Solrock</t>
   </si>
   <si>
-    <t>Nihilego</t>
-  </si>
-  <si>
-    <t>Ultra Abyssmal Cave</t>
-  </si>
-  <si>
-    <t>Buzzwole</t>
-  </si>
-  <si>
-    <t>Pheromosa</t>
-  </si>
-  <si>
-    <t>Xurkitree</t>
-  </si>
-  <si>
-    <t>Celesteela</t>
-  </si>
-  <si>
-    <t>Kartana</t>
-  </si>
-  <si>
-    <t>Guzzlord</t>
-  </si>
-  <si>
-    <t>Poipole</t>
-  </si>
-  <si>
-    <t>Stakataka</t>
-  </si>
-  <si>
-    <t>Blacephalon</t>
-  </si>
-  <si>
     <t>Gligar</t>
   </si>
   <si>
@@ -573,6 +540,21 @@
   </si>
   <si>
     <t>Wooper</t>
+  </si>
+  <si>
+    <t>Pawniard</t>
+  </si>
+  <si>
+    <t>Sandaconda</t>
+  </si>
+  <si>
+    <t>Relic Passage</t>
+  </si>
+  <si>
+    <t>Meowth</t>
+  </si>
+  <si>
+    <t>Dedenne</t>
   </si>
 </sst>
 </file>
@@ -1468,40 +1450,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6</c:v>
@@ -1513,13 +1495,13 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2225,8 +2207,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H86" totalsRowShown="0">
-  <autoFilter ref="B5:H86" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}" name="Tabela1" displayName="Tabela1" ref="B5:H80" totalsRowShown="0">
+  <autoFilter ref="B5:H80" xr:uid="{61C62FF3-7DDB-48A9-9F32-4C197E6D741A}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{CCB72512-45BE-4582-B5B1-F7A9C3F7785B}" name="Pokemon"/>
     <tableColumn id="2" xr3:uid="{2758C6CC-A2DA-4CFB-B52E-6AE39BDC339C}" name="Location"/>
@@ -2542,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M86"/>
+  <dimension ref="B1:M80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,7 +2641,7 @@
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
         <v>139</v>
@@ -2761,22 +2743,22 @@
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>170</v>
       </c>
       <c r="D9" s="5">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E9" t="s">
         <v>141</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" t="s">
         <v>77</v>
@@ -2793,25 +2775,22 @@
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F10" t="s">
-        <v>140</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" t="s">
-        <v>46</v>
+        <v>143</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
       </c>
       <c r="J10" t="s">
         <v>64</v>
@@ -2825,22 +2804,23 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.3</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s">
         <v>140</v>
       </c>
-      <c r="G11" t="s">
-        <v>44</v>
+      <c r="G11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
@@ -2857,13 +2837,13 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>139</v>
       </c>
       <c r="D12" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E12" t="s">
         <v>141</v>
@@ -2889,22 +2869,22 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="D13" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>141</v>
       </c>
       <c r="F13" t="s">
         <v>140</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
         <v>68</v>
@@ -2921,25 +2901,22 @@
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="D14" s="5">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
         <v>140</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J14" t="s">
         <v>72</v>
@@ -2956,43 +2933,48 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D15" s="5">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="E15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F15" t="s">
         <v>140</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.6</v>
+      </c>
       <c r="E16" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="F16" t="s">
         <v>140</v>
       </c>
       <c r="G16" t="s">
         <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>45</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>91</v>
@@ -3003,25 +2985,20 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
         <v>140</v>
       </c>
       <c r="G17" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J17" t="s">
         <v>0</v>
@@ -3038,23 +3015,25 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>145</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.1</v>
+      </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
         <v>140</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>103</v>
       </c>
       <c r="H18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
@@ -3071,25 +3050,23 @@
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C19" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>140</v>
       </c>
       <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
         <v>46</v>
-      </c>
-      <c r="H19" t="s">
-        <v>45</v>
       </c>
       <c r="J19" t="s">
         <v>95</v>
@@ -3106,25 +3083,25 @@
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="D20" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E20" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
         <v>140</v>
       </c>
       <c r="G20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="J20" t="s">
         <v>28</v>
@@ -3141,25 +3118,23 @@
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.15</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="E21" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F21" t="s">
         <v>140</v>
       </c>
       <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
         <v>71</v>
-      </c>
-      <c r="H21" t="s">
-        <v>46</v>
       </c>
       <c r="J21" t="s">
         <v>29</v>
@@ -3176,21 +3151,24 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="D22" s="5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="E22" t="s">
         <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" t="s">
         <v>46</v>
       </c>
       <c r="J22" t="s">
@@ -3208,10 +3186,10 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D23" s="5">
         <v>0.05</v>
@@ -3220,13 +3198,10 @@
         <v>141</v>
       </c>
       <c r="F23" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="J23" t="s">
         <v>31</v>
@@ -3240,23 +3215,25 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="5"/>
+        <v>94</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.05</v>
+      </c>
       <c r="E24" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F24" t="s">
         <v>140</v>
       </c>
       <c r="G24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="J24" t="s">
         <v>27</v>
@@ -3273,25 +3250,23 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
+      <c r="D25" s="5"/>
       <c r="E25" t="s">
         <v>78</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H25" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J25" t="s">
         <v>26</v>
@@ -3305,23 +3280,23 @@
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>158</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" t="s">
         <v>78</v>
       </c>
       <c r="F26" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G26" t="s">
         <v>50</v>
       </c>
       <c r="H26" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J26" t="s">
         <v>36</v>
@@ -3338,25 +3313,23 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
         <v>145</v>
       </c>
-      <c r="D27" s="5">
-        <v>0.05</v>
-      </c>
+      <c r="D27" s="5"/>
       <c r="E27" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
         <v>140</v>
       </c>
       <c r="G27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="J27" t="s">
         <v>58</v>
@@ -3373,13 +3346,13 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>14</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D28" s="5">
-        <v>0.4</v>
+        <v>0.05</v>
       </c>
       <c r="E28" t="s">
         <v>141</v>
@@ -3388,10 +3361,10 @@
         <v>140</v>
       </c>
       <c r="G28" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="J28" t="s">
         <v>79</v>
@@ -3405,19 +3378,25 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>145</v>
+        <v>43</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0.4</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F29" t="s">
         <v>140</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="H29" t="s">
+        <v>52</v>
       </c>
       <c r="J29" t="s">
         <v>80</v>
@@ -3434,25 +3413,19 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0.05</v>
+        <v>145</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F30" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
-      </c>
-      <c r="H30" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="J30" t="s">
         <v>81</v>
@@ -3469,25 +3442,25 @@
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
         <v>109</v>
       </c>
       <c r="D31" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E31" t="s">
         <v>141</v>
       </c>
       <c r="F31" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H31" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J31" t="s">
         <v>82</v>
@@ -3504,23 +3477,25 @@
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
-      </c>
-      <c r="D32" s="5"/>
+        <v>109</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.1</v>
+      </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F32" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="H32" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="J32" t="s">
         <v>83</v>
@@ -3537,7 +3512,7 @@
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
         <v>145</v>
@@ -3567,25 +3542,23 @@
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0.4</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D34" s="5"/>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
         <v>140</v>
       </c>
       <c r="G34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H34" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="J34" t="s">
         <v>85</v>
@@ -3602,25 +3575,25 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D35" s="5">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
         <v>140</v>
       </c>
       <c r="G35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H35" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="J35" t="s">
         <v>86</v>
@@ -3634,10 +3607,10 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D36" s="5">
         <v>0.2</v>
@@ -3649,10 +3622,10 @@
         <v>140</v>
       </c>
       <c r="G36" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="H36" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="J36" t="s">
         <v>87</v>
@@ -3669,22 +3642,25 @@
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="D37" s="5">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
         <v>140</v>
       </c>
       <c r="G37" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
       </c>
       <c r="J37" t="s">
         <v>88</v>
@@ -3701,16 +3677,16 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C38" t="s">
         <v>43</v>
       </c>
       <c r="D38" s="5">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>148</v>
       </c>
       <c r="F38" t="s">
         <v>140</v>
@@ -3718,9 +3694,6 @@
       <c r="G38" t="s">
         <v>49</v>
       </c>
-      <c r="H38" t="s">
-        <v>47</v>
-      </c>
       <c r="J38" t="s">
         <v>89</v>
       </c>
@@ -3733,16 +3706,16 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>126</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
         <v>43</v>
       </c>
       <c r="D39" s="5">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="F39" t="s">
         <v>140</v>
@@ -3750,6 +3723,9 @@
       <c r="G39" t="s">
         <v>49</v>
       </c>
+      <c r="H39" t="s">
+        <v>47</v>
+      </c>
       <c r="J39" t="s">
         <v>90</v>
       </c>
@@ -3765,25 +3741,22 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D40" s="5">
-        <v>0.01</v>
+        <v>0.3</v>
       </c>
       <c r="E40" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="F40" t="s">
         <v>140</v>
       </c>
       <c r="G40" t="s">
-        <v>50</v>
-      </c>
-      <c r="H40" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="J40" t="s">
         <v>40</v>
@@ -3800,13 +3773,13 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>19</v>
+        <v>127</v>
       </c>
       <c r="C41" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D41" s="5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E41" t="s">
         <v>141</v>
@@ -3815,7 +3788,10 @@
         <v>140</v>
       </c>
       <c r="G41" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="H41" t="s">
+        <v>75</v>
       </c>
       <c r="J41" t="s">
         <v>106</v>
@@ -3829,25 +3805,22 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
         <v>140</v>
       </c>
       <c r="G42" t="s">
-        <v>107</v>
-      </c>
-      <c r="H42" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J42" t="s">
         <v>105</v>
@@ -3864,36 +3837,34 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="C43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="5">
-        <v>0.05</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F43" t="s">
         <v>140</v>
       </c>
       <c r="G43" t="s">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="H43" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>125</v>
+        <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
       <c r="D44" s="5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E44" t="s">
         <v>141</v>
@@ -3902,44 +3873,42 @@
         <v>140</v>
       </c>
       <c r="G44" t="s">
-        <v>46</v>
+        <v>54</v>
+      </c>
+      <c r="H44" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
       <c r="C45" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D45" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E45" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F45" t="s">
         <v>140</v>
       </c>
       <c r="G45" t="s">
-        <v>44</v>
-      </c>
-      <c r="H45" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>139</v>
-      </c>
-      <c r="D46" s="5">
-        <v>0.1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D46" s="5"/>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F46" t="s">
         <v>140</v>
@@ -3948,39 +3917,40 @@
         <v>44</v>
       </c>
       <c r="H46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C47" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D47" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F47" t="s">
         <v>140</v>
       </c>
       <c r="G47" t="s">
-        <v>53</v>
+        <v>44</v>
+      </c>
+      <c r="H47" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C48" t="s">
         <v>150</v>
       </c>
-      <c r="D48" s="5">
-        <v>1</v>
-      </c>
+      <c r="D48" s="5"/>
       <c r="E48" t="s">
         <v>78</v>
       </c>
@@ -3988,22 +3958,17 @@
         <v>140</v>
       </c>
       <c r="G48" t="s">
-        <v>55</v>
-      </c>
-      <c r="H48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C49" t="s">
         <v>150</v>
       </c>
-      <c r="D49" s="5">
-        <v>1</v>
-      </c>
+      <c r="D49" s="5"/>
       <c r="E49" t="s">
         <v>78</v>
       </c>
@@ -4011,19 +3976,20 @@
         <v>140</v>
       </c>
       <c r="G49" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="H49" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s">
-        <v>109</v>
-      </c>
-      <c r="D50" s="5">
-        <v>1</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D50" s="5"/>
       <c r="E50" t="s">
         <v>78</v>
       </c>
@@ -4031,19 +3997,17 @@
         <v>140</v>
       </c>
       <c r="G50" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
-      </c>
-      <c r="D51" s="5">
-        <v>1</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D51" s="5"/>
       <c r="E51" t="s">
         <v>78</v>
       </c>
@@ -4051,38 +4015,36 @@
         <v>140</v>
       </c>
       <c r="G51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>145</v>
-      </c>
-      <c r="D52" s="5">
-        <v>0.05</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D52" s="5"/>
       <c r="E52" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F52" t="s">
         <v>140</v>
       </c>
       <c r="G52" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D53" s="5">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="E53" t="s">
         <v>141</v>
@@ -4091,18 +4053,18 @@
         <v>140</v>
       </c>
       <c r="G53" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D54" s="5">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="E54" t="s">
         <v>141</v>
@@ -4111,38 +4073,35 @@
         <v>140</v>
       </c>
       <c r="G54" t="s">
-        <v>75</v>
-      </c>
-      <c r="H54" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>40</v>
+        <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D55" s="5">
-        <v>0.15</v>
+        <v>0.3</v>
       </c>
       <c r="E55" t="s">
         <v>141</v>
       </c>
       <c r="F55" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G55" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="H55" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C56" t="s">
         <v>43</v>
@@ -4154,67 +4113,67 @@
         <v>141</v>
       </c>
       <c r="F56" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G56" t="s">
+        <v>46</v>
+      </c>
+      <c r="H56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D57" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>141</v>
+      </c>
+      <c r="F57" t="s">
+        <v>140</v>
+      </c>
+      <c r="G57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D57" s="10">
+      <c r="D58" s="10">
         <v>0.2</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G57" s="2" t="s">
+      <c r="E58" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G58" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" t="s">
-        <v>149</v>
-      </c>
-      <c r="D58" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="E58" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" t="s">
-        <v>140</v>
-      </c>
-      <c r="G58" t="s">
-        <v>55</v>
-      </c>
-      <c r="H58" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="D59" s="5">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E59" t="s">
         <v>141</v>
@@ -4223,18 +4182,21 @@
         <v>140</v>
       </c>
       <c r="G59" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="H59" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="C60" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="D60" s="5">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="E60" t="s">
         <v>141</v>
@@ -4243,61 +4205,61 @@
         <v>140</v>
       </c>
       <c r="G60" t="s">
-        <v>97</v>
-      </c>
-      <c r="H60" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D61" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E61" t="s">
         <v>141</v>
       </c>
       <c r="F61" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G61" t="s">
-        <v>75</v>
+        <v>97</v>
+      </c>
+      <c r="H61" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
       <c r="C62" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="D62" s="5">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="E62" t="s">
         <v>141</v>
       </c>
       <c r="F62" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="D63" s="5">
-        <v>0.3</v>
+        <v>0.04</v>
       </c>
       <c r="E63" t="s">
         <v>141</v>
@@ -4306,18 +4268,18 @@
         <v>140</v>
       </c>
       <c r="G63" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D64" s="5">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="E64" t="s">
         <v>141</v>
@@ -4326,18 +4288,18 @@
         <v>140</v>
       </c>
       <c r="G64" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="D65" s="5">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E65" t="s">
         <v>141</v>
@@ -4346,21 +4308,18 @@
         <v>140</v>
       </c>
       <c r="G65" t="s">
-        <v>49</v>
-      </c>
-      <c r="H65" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="C66" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="D66" s="5">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="E66" t="s">
         <v>141</v>
@@ -4369,18 +4328,21 @@
         <v>140</v>
       </c>
       <c r="G66" t="s">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="H66" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D67" s="5">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="E67" t="s">
         <v>141</v>
@@ -4389,18 +4351,18 @@
         <v>140</v>
       </c>
       <c r="G67" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
         <v>146</v>
       </c>
       <c r="D68" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E68" t="s">
         <v>141</v>
@@ -4414,10 +4376,10 @@
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="C69" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="5">
         <v>0.1</v>
@@ -4429,18 +4391,15 @@
         <v>140</v>
       </c>
       <c r="G69" t="s">
-        <v>46</v>
-      </c>
-      <c r="H69" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="C70" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="D70" s="5">
         <v>0.1</v>
@@ -4452,24 +4411,22 @@
         <v>140</v>
       </c>
       <c r="G70" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="H70" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>43</v>
-      </c>
-      <c r="D71" s="5">
-        <v>0.1</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D71" s="5"/>
       <c r="E71" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F71" t="s">
         <v>140</v>
@@ -4478,41 +4435,41 @@
         <v>52</v>
       </c>
       <c r="H71" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>48</v>
+        <v>117</v>
       </c>
       <c r="C72" t="s">
         <v>43</v>
       </c>
       <c r="D72" s="5">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E72" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F72" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G72" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H72" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C73" t="s">
-        <v>146</v>
+        <v>43</v>
       </c>
       <c r="D73" s="5">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="E73" t="s">
         <v>141</v>
@@ -4521,41 +4478,42 @@
         <v>140</v>
       </c>
       <c r="G73" t="s">
-        <v>71</v>
+        <v>52</v>
+      </c>
+      <c r="H73" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>174</v>
+        <v>48</v>
       </c>
       <c r="C74" t="s">
-        <v>142</v>
-      </c>
-      <c r="D74" s="5">
-        <v>0.05</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D74" s="5"/>
       <c r="E74" t="s">
-        <v>141</v>
+        <v>78</v>
       </c>
       <c r="F74" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G74" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="H74" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>112</v>
+        <v>172</v>
       </c>
       <c r="C75" t="s">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="D75" s="5">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E75" t="s">
         <v>141</v>
@@ -4564,227 +4522,116 @@
         <v>140</v>
       </c>
       <c r="G75" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="H75" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C76" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="D76" s="5">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="E76" t="s">
         <v>141</v>
       </c>
       <c r="F76" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G76" t="s">
-        <v>46</v>
-      </c>
-      <c r="H76" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>163</v>
+        <v>142</v>
+      </c>
+      <c r="D77" s="5">
+        <v>0.05</v>
       </c>
       <c r="E77" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F77" t="s">
         <v>140</v>
       </c>
       <c r="G77" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="H77" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>164</v>
+        <v>112</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
+        <v>94</v>
+      </c>
+      <c r="D78" s="5">
+        <v>0.2</v>
       </c>
       <c r="E78" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F78" t="s">
         <v>140</v>
       </c>
       <c r="G78" t="s">
-        <v>97</v>
-      </c>
-      <c r="H78" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>163</v>
+        <v>109</v>
+      </c>
+      <c r="D79" s="5">
+        <v>0.1</v>
       </c>
       <c r="E79" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F79" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G79" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="H79" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C80" t="s">
-        <v>163</v>
+        <v>170</v>
+      </c>
+      <c r="D80" s="5">
+        <v>0.3</v>
       </c>
       <c r="E80" t="s">
-        <v>78</v>
+        <v>141</v>
       </c>
       <c r="F80" t="s">
         <v>140</v>
       </c>
       <c r="G80" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>167</v>
-      </c>
-      <c r="C81" t="s">
-        <v>163</v>
-      </c>
-      <c r="E81" t="s">
-        <v>78</v>
-      </c>
-      <c r="F81" t="s">
-        <v>140</v>
-      </c>
-      <c r="G81" t="s">
-        <v>50</v>
-      </c>
-      <c r="H81" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>168</v>
-      </c>
-      <c r="C82" t="s">
-        <v>163</v>
-      </c>
-      <c r="E82" t="s">
-        <v>78</v>
-      </c>
-      <c r="F82" t="s">
-        <v>140</v>
-      </c>
-      <c r="G82" t="s">
-        <v>53</v>
-      </c>
-      <c r="H82" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>169</v>
-      </c>
-      <c r="C83" t="s">
-        <v>163</v>
-      </c>
-      <c r="E83" t="s">
-        <v>78</v>
-      </c>
-      <c r="F83" t="s">
-        <v>140</v>
-      </c>
-      <c r="G83" t="s">
-        <v>52</v>
-      </c>
-      <c r="H83" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>170</v>
-      </c>
-      <c r="C84" t="s">
-        <v>163</v>
-      </c>
-      <c r="E84" t="s">
-        <v>78</v>
-      </c>
-      <c r="F84" t="s">
-        <v>140</v>
-      </c>
-      <c r="G84" t="s">
-        <v>44</v>
-      </c>
-      <c r="H84" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>171</v>
-      </c>
-      <c r="C85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E85" t="s">
-        <v>78</v>
-      </c>
-      <c r="F85" t="s">
-        <v>140</v>
-      </c>
-      <c r="G85" t="s">
-        <v>47</v>
-      </c>
-      <c r="H85" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" t="s">
-        <v>163</v>
-      </c>
-      <c r="E86" t="s">
-        <v>78</v>
-      </c>
-      <c r="F86" t="s">
-        <v>140</v>
-      </c>
-      <c r="G86" t="s">
-        <v>55</v>
-      </c>
-      <c r="H86" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -4809,7 +4656,7 @@
   <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,7 +4711,7 @@
       </c>
       <c r="C5">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -4873,7 +4720,7 @@
       </c>
       <c r="C6">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
@@ -4882,7 +4729,7 @@
       </c>
       <c r="C7">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
@@ -4891,7 +4738,7 @@
       </c>
       <c r="C8">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
@@ -4900,7 +4747,7 @@
       </c>
       <c r="C9">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
@@ -4909,7 +4756,7 @@
       </c>
       <c r="C10">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -4918,7 +4765,7 @@
       </c>
       <c r="C11">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -4927,7 +4774,7 @@
       </c>
       <c r="C12">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
@@ -4936,7 +4783,7 @@
       </c>
       <c r="C13">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -4945,7 +4792,7 @@
       </c>
       <c r="C14">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -4963,7 +4810,7 @@
       </c>
       <c r="C16">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -4999,7 +4846,7 @@
       </c>
       <c r="C20">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -5017,7 +4864,7 @@
       </c>
       <c r="C22">
         <f>COUNTIF(Tabela1[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela2[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]]) + COUNTIF(Tabela4[[Type 1]:[Type 2]],Tabela3[[#This Row],[Type]])</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>